<commit_message>
correct signaldb excel, frame to signal works, ros signal publisher callback now connected
</commit_message>
<xml_diff>
--- a/signaldb.xlsx
+++ b/signaldb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Signals" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="166">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -135,15 +135,12 @@
     <t xml:space="preserve">Car Speed</t>
   </si>
   <si>
-    <t xml:space="preserve">a</t>
+    <t xml:space="preserve">Signed</t>
   </si>
   <si>
     <t xml:space="preserve">Car TurnRate</t>
   </si>
   <si>
-    <t xml:space="preserve">Signed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Speed Request Speed</t>
   </si>
   <si>
@@ -486,24 +483,36 @@
     <t xml:space="preserve">0x16</t>
   </si>
   <si>
+    <t xml:space="preserve">56,57,58</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gyro</t>
   </si>
   <si>
     <t xml:space="preserve">0x17</t>
   </si>
   <si>
+    <t xml:space="preserve">59,60,61</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accelerometer</t>
   </si>
   <si>
     <t xml:space="preserve">0x18</t>
   </si>
   <si>
+    <t xml:space="preserve">62,63,64</t>
+  </si>
+  <si>
     <t xml:space="preserve">Magnetometer</t>
   </si>
   <si>
     <t xml:space="preserve">0x19</t>
   </si>
   <si>
+    <t xml:space="preserve">67,68,69</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heartbeat VCU</t>
   </si>
   <si>
@@ -511,15 +520,6 @@
   </si>
   <si>
     <t xml:space="preserve">HB and status from VCU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heartbeat BMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HB and status from BMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Enable</t>
   </si>
 </sst>
 </file>
@@ -670,8 +670,8 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,7 +1238,7 @@
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>16</v>
@@ -1261,10 +1261,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>16</v>
@@ -1279,7 +1279,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,10 +1287,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>16</v>
@@ -1305,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,10 +1313,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>16</v>
@@ -1336,10 +1336,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>16</v>
@@ -1359,7 +1359,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>10</v>
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1385,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
@@ -1400,10 +1400,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,7 +1411,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
@@ -1426,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,7 +1437,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>10</v>
@@ -1452,10 +1452,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,7 +1463,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
@@ -1486,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>10</v>
@@ -1509,7 +1509,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>10</v>
@@ -1532,7 +1532,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>10</v>
@@ -1555,7 +1555,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -1570,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
@@ -1593,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1601,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
@@ -1616,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,7 +1624,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>10</v>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,7 +1647,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>10</v>
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1670,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>10</v>
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,7 +1693,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>10</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1716,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>20</v>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1739,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>10</v>
@@ -1765,7 +1765,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>10</v>
@@ -1791,10 +1791,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>8</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,10 +1814,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>8</v>
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,10 +1837,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" s="3" t="n">
         <v>8</v>
@@ -1860,10 +1860,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="3" t="n">
         <v>8</v>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,10 +1883,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D49" s="3" t="n">
         <v>8</v>
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,10 +1906,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50" s="3" t="n">
         <v>8</v>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,10 +1929,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" s="3" t="n">
         <v>8</v>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,10 +1952,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D52" s="3" t="n">
         <v>8</v>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1975,10 +1975,10 @@
         <v>56</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>16</v>
@@ -1992,7 +1992,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,10 +2000,10 @@
         <v>57</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>16</v>
@@ -2017,7 +2017,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,10 +2025,10 @@
         <v>58</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>16</v>
@@ -2042,7 +2042,7 @@
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,10 +2050,10 @@
         <v>59</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>16</v>
@@ -2067,7 +2067,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2075,10 +2075,10 @@
         <v>60</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D57" s="5" t="n">
         <v>16</v>
@@ -2092,7 +2092,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2100,10 +2100,10 @@
         <v>61</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>16</v>
@@ -2117,7 +2117,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2125,10 +2125,10 @@
         <v>62</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D59" s="5" t="n">
         <v>16</v>
@@ -2142,7 +2142,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2150,10 +2150,10 @@
         <v>63</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>16</v>
@@ -2167,7 +2167,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2175,10 +2175,10 @@
         <v>64</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D61" s="5" t="n">
         <v>16</v>
@@ -2192,7 +2192,7 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2200,7 +2200,7 @@
         <v>65</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>10</v>
@@ -2217,7 +2217,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2225,7 +2225,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>10</v>
@@ -2242,7 +2242,7 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2250,10 +2250,10 @@
         <v>67</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D64" s="5" t="n">
         <v>16</v>
@@ -2267,7 +2267,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2275,10 +2275,10 @@
         <v>68</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D65" s="5" t="n">
         <v>16</v>
@@ -2292,7 +2292,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2300,10 +2300,10 @@
         <v>69</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D66" s="5" t="n">
         <v>16</v>
@@ -2317,7 +2317,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2336,10 +2336,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2352,19 +2352,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -2372,286 +2372,286 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>48</v>
@@ -2660,21 +2660,21 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>52</v>
@@ -2683,21 +2683,21 @@
         <v>0.1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>54</v>
@@ -2706,30 +2706,30 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C17" s="5" t="n">
-        <v>56</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>0.1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="6" t="n">
         <v>1</v>
@@ -2737,19 +2737,19 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>57</v>
+        <v>155</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" s="6" t="n">
         <v>1</v>
@@ -2757,19 +2757,19 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>58</v>
+        <v>158</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="6" t="n">
         <v>1</v>
@@ -2777,184 +2777,32 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>59</v>
+        <v>161</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>0.01</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="D21" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>61</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>62</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>63</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>67</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>68</v>
-      </c>
-      <c r="D27" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="D28" s="5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2971,10 +2819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2987,19 +2835,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -3007,13 +2855,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.01</v>
@@ -3025,18 +2873,18 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.01</v>
@@ -3048,18 +2896,18 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.01</v>
@@ -3071,18 +2919,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.01</v>
@@ -3094,18 +2942,18 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0.01</v>
@@ -3117,18 +2965,18 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.01</v>
@@ -3140,41 +2988,41 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.01</v>
@@ -3186,18 +3034,18 @@
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -3209,77 +3057,57 @@
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>163</v>
+        <v>138</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>